<commit_message>
Read Attack Payload from files
</commit_message>
<xml_diff>
--- a/mooncore-Security/Datas/MUS.xlsx
+++ b/mooncore-Security/Datas/MUS.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Headers</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>shabana1@mailinator.com</t>
   </si>
   <si>
     <t>Philips@1</t>
@@ -112,7 +109,13 @@
     <t>FUZZFULL,SQL,XSS,HTTPVERB</t>
   </si>
   <si>
-    <t>HTTPVERB</t>
+    <t>FULLFUZZ</t>
+  </si>
+  <si>
+    <t>auth,methodType</t>
+  </si>
+  <si>
+    <t>FUZZFULL,HTTPVERB</t>
   </si>
 </sst>
 </file>
@@ -473,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -503,45 +506,45 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -566,7 +569,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -579,53 +582,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -640,76 +640,61 @@
     <col min="8" max="8" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="C4" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -723,57 +708,42 @@
     <col min="7" max="7" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>